<commit_message>
Update for Weekly and budget
</commit_message>
<xml_diff>
--- a/mobile.xlsx
+++ b/mobile.xlsx
@@ -132,13 +132,13 @@
         <v>0.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1535978.0</v>
+        <v>1799033.0</v>
       </c>
       <c r="D2" t="n">
-        <v>7907.0</v>
+        <v>8177.0</v>
       </c>
       <c r="E2" t="n">
-        <v>108.702459</v>
+        <v>114.530322</v>
       </c>
       <c r="F2" t="n">
         <v>0.0</v>
@@ -161,13 +161,13 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>895809.0</v>
+        <v>1269916.0</v>
       </c>
       <c r="D3" t="n">
-        <v>3690.0</v>
+        <v>3619.0</v>
       </c>
       <c r="E3" t="n">
-        <v>63.502809</v>
+        <v>67.913795</v>
       </c>
       <c r="F3" t="n">
         <v>0.0</v>

</xml_diff>